<commit_message>
set value to zero where filter applies
</commit_message>
<xml_diff>
--- a/input/test.xlsx
+++ b/input/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t xml:space="preserve">column A1</t>
   </si>
@@ -84,175 +84,178 @@
     <t>1,31</t>
   </si>
   <si>
+    <t>qwertz</t>
+  </si>
+  <si>
+    <t>1,32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 11</t>
+  </si>
+  <si>
+    <t>1,33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">string 10</t>
   </si>
   <si>
-    <t>1,32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 11</t>
-  </si>
-  <si>
-    <t>1,33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 17</t>
-  </si>
-  <si>
     <t xml:space="preserve">string 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string 6</t>
   </si>
 </sst>
 </file>
@@ -294,15 +297,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -912,7 +912,7 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6">
@@ -929,7 +929,7 @@
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7">
@@ -988,7 +988,7 @@
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C11">
@@ -1083,7 +1083,7 @@
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>111128</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20">
         <v>111129</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21">
         <v>111130</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>111131</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23">
         <v>111132</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>111133</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>111134</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26">
         <v>111135</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27">
         <v>111136</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28">
         <v>111137</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29">
         <v>111138</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="30" ht="14.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>111139</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31">
         <v>111140</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32">
         <v>111141</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33">
         <v>111142</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34">
         <v>111143</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="35" ht="14.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35">
         <v>111144</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36">
         <v>111145</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37">
         <v>111146</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38">
         <v>111147</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39">
         <v>111148</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40">
         <v>111149</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="41" ht="14.25">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41">
         <v>111150</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42">
         <v>111151</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43">
         <v>111152</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="44" ht="14.25">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C44">
         <v>111153</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="45" ht="14.25">
       <c r="A45" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45">
         <v>111154</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="46" ht="14.25">
       <c r="A46" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46">
         <v>111155</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="47" ht="14.25">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47">
         <v>111156</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="48" ht="14.25">
       <c r="A48" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48">
         <v>111157</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49">
         <v>111158</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="50" ht="14.25">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50">
         <v>111159</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="51" ht="14.25">
       <c r="A51" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51">
         <v>111160</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52">
         <v>111161</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="53" ht="14.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53">
         <v>111162</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="54" ht="14.25">
       <c r="A54" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54">
         <v>111163</v>
@@ -1479,7 +1479,7 @@
     </row>
     <row r="55" ht="14.25">
       <c r="A55" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55">
         <v>111164</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="56" ht="14.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56">
         <v>111165</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="57" ht="14.25">
       <c r="A57" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57">
         <v>111166</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="58" ht="14.25">
       <c r="A58" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58">
         <v>111167</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="59" ht="14.25">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59">
         <v>111168</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="60" ht="14.25">
       <c r="A60" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60">
         <v>111169</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="61" ht="14.25">
       <c r="A61" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61">
         <v>111170</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="62" ht="14.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62">
         <v>111171</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="63" ht="14.25">
       <c r="A63" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63">
         <v>111172</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="68" ht="14.25">
       <c r="A68" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68">
         <v>111177</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="69" ht="14.25">
       <c r="A69" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69">
         <v>111178</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C73">
         <v>111182</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="81" ht="14.25">
       <c r="A81" s="5" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C81">
         <v>111190</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="82" ht="14.25">
       <c r="A82" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C82">
         <v>111191</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="83" ht="14.25">
       <c r="A83" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C83">
         <v>111192</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C84">
         <v>111193</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C85">
         <v>111194</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C86">
         <v>111195</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C87">
         <v>111196</v>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="88" ht="14.25">
       <c r="A88" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C88">
         <v>111197</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="89" ht="14.25">
       <c r="A89" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C89">
         <v>111198</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="90" ht="14.25">
       <c r="A90" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C90">
         <v>111199</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="91" ht="14.25">
       <c r="A91" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C91">
         <v>111200</v>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C92">
         <v>111201</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C93">
         <v>111202</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="94" ht="14.25">
       <c r="A94" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C94">
         <v>111203</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="95" ht="14.25">
       <c r="A95" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C95">
         <v>111204</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="96" ht="14.25">
       <c r="A96" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C96">
         <v>111205</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="97" ht="14.25">
       <c r="A97" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C97">
         <v>111206</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="98" ht="14.25">
       <c r="A98" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C98">
         <v>111207</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="99" ht="14.25">
       <c r="A99" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C99">
         <v>111208</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="100" ht="14.25">
       <c r="A100" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C100">
         <v>111209</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="101" ht="14.25">
       <c r="A101" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C101">
         <v>111210</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C102">
         <v>111211</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="103" ht="14.25">
       <c r="A103" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C103">
         <v>111212</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C104">
         <v>111213</v>
@@ -2029,7 +2029,7 @@
     </row>
     <row r="105" ht="14.25">
       <c r="A105" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C105">
         <v>111214</v>
@@ -2040,7 +2040,7 @@
     </row>
     <row r="106" ht="14.25">
       <c r="A106" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C106">
         <v>111215</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C107">
         <v>111216</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C108">
         <v>111217</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C109">
         <v>111218</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C110">
         <v>111219</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C111">
         <v>111220</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C112">
         <v>111221</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C113">
         <v>111222</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C114">
         <v>111223</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C115">
         <v>111224</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C116" s="5">
         <v>111111</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C117" s="5">
         <v>111112</v>
@@ -2172,7 +2172,7 @@
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C118" s="5">
         <v>111113</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C119" s="5">
         <v>111114</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C120" s="5">
         <v>111115</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C121" s="5">
         <v>111116</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C122" s="5">
         <v>111117</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="123" ht="14.25">
       <c r="A123" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C123" s="5">
         <v>111118</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="124" ht="14.25">
       <c r="A124" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C124" s="5">
         <v>111119</v>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="125" ht="14.25">
       <c r="A125" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C125" s="5">
         <v>111120</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="130" ht="14.25">
       <c r="A130" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C130" s="5">
         <v>111125</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="131" ht="14.25">
       <c r="A131" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C131" s="5">
         <v>111126</v>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="135" ht="14.25">
       <c r="A135" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C135" s="5">
         <v>111130</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="143" ht="14.25">
       <c r="A143" s="5" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C143" s="5">
         <v>111138</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="144" ht="14.25">
       <c r="A144" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C144" s="5">
         <v>111139</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="145" ht="14.25">
       <c r="A145" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C145" s="5">
         <v>111140</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="146" ht="14.25">
       <c r="A146" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C146" s="5">
         <v>111141</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="147" ht="14.25">
       <c r="A147" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C147" s="5">
         <v>111142</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="148" ht="14.25">
       <c r="A148" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C148" s="5">
         <v>111143</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="149" ht="14.25">
       <c r="A149" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C149" s="5">
         <v>111144</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="150" ht="14.25">
       <c r="A150" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C150" s="5">
         <v>111145</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="151" ht="14.25">
       <c r="A151" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C151" s="5">
         <v>111146</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="152" ht="14.25">
       <c r="A152" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C152" s="5">
         <v>111147</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="153" ht="14.25">
       <c r="A153" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C153" s="5">
         <v>111148</v>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="154" ht="14.25">
       <c r="A154" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C154" s="5">
         <v>111149</v>
@@ -2578,7 +2578,7 @@
       </c>
     </row>
     <row r="155" ht="14.25">
-      <c r="A155" s="4" t="s">
+      <c r="A155" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C155" s="5">
@@ -2589,7 +2589,7 @@
       </c>
     </row>
     <row r="156" ht="14.25">
-      <c r="A156" s="4" t="s">
+      <c r="A156" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C156" s="5">
@@ -2600,7 +2600,7 @@
       </c>
     </row>
     <row r="157" ht="14.25">
-      <c r="A157" s="4" t="s">
+      <c r="A157" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C157" s="5">
@@ -2611,7 +2611,7 @@
       </c>
     </row>
     <row r="158" ht="14.25">
-      <c r="A158" s="4" t="s">
+      <c r="A158" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C158" s="5">
@@ -2622,7 +2622,7 @@
       </c>
     </row>
     <row r="159" ht="14.25">
-      <c r="A159" s="4" t="s">
+      <c r="A159" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C159" s="5">
@@ -2633,7 +2633,7 @@
       </c>
     </row>
     <row r="160" ht="14.25">
-      <c r="A160" s="4" t="s">
+      <c r="A160" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C160" s="5">
@@ -2645,7 +2645,7 @@
     </row>
     <row r="161" ht="14.25">
       <c r="A161" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C161" s="5">
         <v>111156</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="162" ht="14.25">
       <c r="A162" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C162" s="5">
         <v>111157</v>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="163" ht="14.25">
       <c r="A163" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C163" s="5">
         <v>111158</v>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="164" ht="14.25">
       <c r="A164" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C164" s="5">
         <v>111159</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="165" ht="14.25">
       <c r="A165" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C165" s="5">
         <v>111160</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="166" ht="14.25">
       <c r="A166" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C166" s="5">
         <v>111161</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="167" ht="14.25">
       <c r="A167" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C167" s="5">
         <v>111162</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="168" ht="14.25">
       <c r="A168" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C168" s="5">
         <v>111163</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="169" ht="14.25">
       <c r="A169" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C169" s="5">
         <v>111164</v>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="170" ht="14.25">
       <c r="A170" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C170" s="5">
         <v>111165</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="171" ht="14.25">
       <c r="A171" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C171" s="5">
         <v>111166</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="172" ht="14.25">
       <c r="A172" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C172" s="5">
         <v>111167</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="173" ht="14.25">
       <c r="A173" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C173" s="5">
         <v>111168</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="174" ht="14.25">
       <c r="A174" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C174" s="5">
         <v>111169</v>
@@ -2799,7 +2799,7 @@
     </row>
     <row r="175" ht="14.25">
       <c r="A175" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C175" s="5">
         <v>111170</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="176" ht="14.25">
       <c r="A176" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C176" s="5">
         <v>111171</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="177" ht="14.25">
       <c r="A177" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C177" s="5">
         <v>111172</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="178" ht="14.25">
       <c r="A178" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C178" s="5">
         <v>111173</v>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="179" ht="14.25">
       <c r="A179" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C179" s="5">
         <v>111174</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="180" ht="14.25">
       <c r="A180" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C180" s="5">
         <v>111175</v>
@@ -2865,7 +2865,7 @@
     </row>
     <row r="181" ht="14.25">
       <c r="A181" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C181" s="5">
         <v>111176</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="182" ht="14.25">
       <c r="A182" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C182" s="5">
         <v>111177</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="183" ht="14.25">
       <c r="A183" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C183" s="5">
         <v>111178</v>
@@ -2898,7 +2898,7 @@
     </row>
     <row r="184" ht="14.25">
       <c r="A184" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C184" s="5">
         <v>111179</v>
@@ -2909,7 +2909,7 @@
     </row>
     <row r="185" ht="14.25">
       <c r="A185" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C185" s="5">
         <v>111180</v>
@@ -2920,7 +2920,7 @@
     </row>
     <row r="186" ht="14.25">
       <c r="A186" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C186" s="5">
         <v>111181</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="187" ht="14.25">
       <c r="A187" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C187" s="5">
         <v>111182</v>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="192" ht="14.25">
       <c r="A192" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C192" s="5">
         <v>111187</v>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="193" ht="14.25">
       <c r="A193" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C193" s="5">
         <v>111188</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="197" ht="14.25">
       <c r="A197" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C197" s="5">
         <v>111192</v>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="205" ht="14.25">
       <c r="A205" s="5" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C205" s="5">
         <v>111200</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="206" ht="14.25">
       <c r="A206" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C206" s="5">
         <v>111201</v>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="207" ht="14.25">
       <c r="A207" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C207" s="5">
         <v>111202</v>
@@ -3162,7 +3162,7 @@
     </row>
     <row r="208" ht="14.25">
       <c r="A208" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C208" s="5">
         <v>111203</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="209" ht="14.25">
       <c r="A209" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C209" s="5">
         <v>111204</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="210" ht="14.25">
       <c r="A210" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C210" s="5">
         <v>111205</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="211" ht="14.25">
       <c r="A211" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C211" s="5">
         <v>111206</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="212" ht="14.25">
       <c r="A212" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C212" s="5">
         <v>111207</v>
@@ -3217,7 +3217,7 @@
     </row>
     <row r="213" ht="14.25">
       <c r="A213" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C213" s="5">
         <v>111208</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="214" ht="14.25">
       <c r="A214" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C214" s="5">
         <v>111209</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="215" ht="14.25">
       <c r="A215" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C215" s="5">
         <v>111210</v>
@@ -3250,7 +3250,7 @@
     </row>
     <row r="216" ht="14.25">
       <c r="A216" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C216" s="5">
         <v>111211</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="217" ht="14.25">
       <c r="A217" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C217" s="5">
         <v>111212</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="218" ht="14.25">
       <c r="A218" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C218" s="5">
         <v>111213</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="219" ht="14.25">
       <c r="A219" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C219" s="5">
         <v>111214</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="220" ht="14.25">
       <c r="A220" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C220" s="5">
         <v>111215</v>
@@ -3305,7 +3305,7 @@
     </row>
     <row r="221" ht="14.25">
       <c r="A221" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C221" s="5">
         <v>111216</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="222" ht="14.25">
       <c r="A222" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C222" s="5">
         <v>111217</v>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="223" ht="14.25">
       <c r="A223" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C223" s="5">
         <v>111218</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="224" ht="14.25">
       <c r="A224" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C224" s="5">
         <v>111219</v>
@@ -3349,7 +3349,7 @@
     </row>
     <row r="225" ht="14.25">
       <c r="A225" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C225" s="5">
         <v>111220</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="226" ht="14.25">
       <c r="A226" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C226" s="5">
         <v>111221</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="227" ht="14.25">
       <c r="A227" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C227" s="5">
         <v>111222</v>
@@ -3382,7 +3382,7 @@
     </row>
     <row r="228" ht="14.25">
       <c r="A228" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C228" s="5">
         <v>111223</v>
@@ -3393,7 +3393,7 @@
     </row>
     <row r="229" ht="14.25">
       <c r="A229" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C229" s="5">
         <v>111224</v>
@@ -3404,7 +3404,7 @@
     </row>
     <row r="230" ht="14.25">
       <c r="A230" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C230">
         <v>888888</v>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="231" ht="14.25">
       <c r="A231" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C231">
         <v>888889</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="232" ht="14.25">
       <c r="A232" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C232">
         <v>888890</v>
@@ -3437,7 +3437,7 @@
     </row>
     <row r="233" ht="14.25">
       <c r="A233" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C233">
         <v>888891</v>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="234" ht="14.25">
       <c r="A234" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C234">
         <v>888892</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="235" ht="14.25">
       <c r="A235" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C235">
         <v>888893</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="236" ht="14.25">
       <c r="A236" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C236">
         <v>888894</v>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="237" ht="14.25">
       <c r="A237" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C237">
         <v>888895</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="238" ht="14.25">
       <c r="A238" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C238">
         <v>888896</v>
@@ -3503,7 +3503,7 @@
     </row>
     <row r="239" ht="14.25">
       <c r="A239" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C239">
         <v>888897</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="240" ht="14.25">
       <c r="A240" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C240">
         <v>888898</v>
@@ -3525,7 +3525,7 @@
     </row>
     <row r="241" ht="14.25">
       <c r="A241" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C241">
         <v>888899</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="242" ht="14.25">
       <c r="A242" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C242">
         <v>888900</v>
@@ -3547,7 +3547,7 @@
     </row>
     <row r="243" ht="14.25">
       <c r="A243" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C243">
         <v>888901</v>
@@ -3558,7 +3558,7 @@
     </row>
     <row r="244" ht="14.25">
       <c r="A244" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C244">
         <v>888902</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="245" ht="14.25">
       <c r="A245" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C245">
         <v>888903</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="246" ht="14.25">
       <c r="A246" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C246">
         <v>888904</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="247" ht="14.25">
       <c r="A247" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C247">
         <v>888905</v>
@@ -3602,7 +3602,7 @@
     </row>
     <row r="248" ht="14.25">
       <c r="A248" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C248">
         <v>888906</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="249" ht="14.25">
       <c r="A249" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C249">
         <v>888907</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="254" ht="14.25">
       <c r="A254" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C254">
         <v>888912</v>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="255" ht="14.25">
       <c r="A255" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C255">
         <v>888913</v>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="259" ht="14.25">
       <c r="A259" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C259">
         <v>888917</v>
@@ -3811,7 +3811,7 @@
     </row>
     <row r="267" ht="14.25">
       <c r="A267" s="5" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C267">
         <v>888925</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="268" ht="14.25">
       <c r="A268" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C268">
         <v>888926</v>
@@ -3833,7 +3833,7 @@
     </row>
     <row r="269" ht="14.25">
       <c r="A269" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C269">
         <v>888927</v>
@@ -3844,7 +3844,7 @@
     </row>
     <row r="270" ht="14.25">
       <c r="A270" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C270">
         <v>888928</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="271" ht="14.25">
       <c r="A271" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C271">
         <v>888929</v>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="272" ht="14.25">
       <c r="A272" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C272">
         <v>888930</v>
@@ -3877,7 +3877,7 @@
     </row>
     <row r="273" ht="14.25">
       <c r="A273" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C273">
         <v>888931</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="274" ht="14.25">
       <c r="A274" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C274">
         <v>888932</v>
@@ -3899,7 +3899,7 @@
     </row>
     <row r="275" ht="14.25">
       <c r="A275" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C275">
         <v>888933</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="276" ht="14.25">
       <c r="A276" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C276">
         <v>888934</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="277" ht="14.25">
       <c r="A277" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C277">
         <v>888935</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="278" ht="14.25">
       <c r="A278" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C278">
         <v>888936</v>
@@ -3943,7 +3943,7 @@
     </row>
     <row r="279" ht="14.25">
       <c r="A279" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C279">
         <v>888937</v>
@@ -3954,7 +3954,7 @@
     </row>
     <row r="280" ht="14.25">
       <c r="A280" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C280">
         <v>888938</v>
@@ -3965,7 +3965,7 @@
     </row>
     <row r="281" ht="14.25">
       <c r="A281" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C281">
         <v>888939</v>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="282" ht="14.25">
       <c r="A282" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C282">
         <v>888940</v>
@@ -3987,7 +3987,7 @@
     </row>
     <row r="283" ht="14.25">
       <c r="A283" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C283">
         <v>888941</v>
@@ -3998,7 +3998,7 @@
     </row>
     <row r="284" ht="14.25">
       <c r="A284" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C284">
         <v>888942</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="285" ht="14.25">
       <c r="A285" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C285">
         <v>888943</v>
@@ -4020,7 +4020,7 @@
     </row>
     <row r="286" ht="14.25">
       <c r="A286" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C286">
         <v>888944</v>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="287" ht="14.25">
       <c r="A287" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C287">
         <v>888945</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="288" ht="14.25">
       <c r="A288" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C288">
         <v>888946</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="289" ht="14.25">
       <c r="A289" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C289">
         <v>888947</v>
@@ -4064,7 +4064,7 @@
     </row>
     <row r="290" ht="14.25">
       <c r="A290" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C290">
         <v>888948</v>
@@ -4075,7 +4075,7 @@
     </row>
     <row r="291" ht="14.25">
       <c r="A291" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C291">
         <v>888949</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="292" ht="14.25">
       <c r="A292" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C292">
         <v>888950</v>
@@ -4096,7 +4096,7 @@
       </c>
     </row>
     <row r="293" ht="14.25">
-      <c r="A293" s="4" t="s">
+      <c r="A293" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C293">
@@ -4107,7 +4107,7 @@
       </c>
     </row>
     <row r="294" ht="14.25">
-      <c r="A294" s="4" t="s">
+      <c r="A294" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C294">
@@ -4118,7 +4118,7 @@
       </c>
     </row>
     <row r="295" ht="14.25">
-      <c r="A295" s="6" t="s">
+      <c r="A295" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C295">
@@ -4130,7 +4130,7 @@
     </row>
     <row r="296" ht="14.25">
       <c r="A296" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C296">
         <v>888954</v>
@@ -4141,7 +4141,7 @@
     </row>
     <row r="297" ht="14.25">
       <c r="A297" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C297">
         <v>888955</v>
@@ -4152,7 +4152,7 @@
     </row>
     <row r="298" ht="14.25">
       <c r="A298" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C298">
         <v>888956</v>
@@ -4163,7 +4163,7 @@
     </row>
     <row r="299" ht="14.25">
       <c r="A299" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C299">
         <v>888957</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="300" ht="14.25">
       <c r="A300" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C300">
         <v>888958</v>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="301" ht="14.25">
       <c r="A301" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C301" s="5">
         <v>111111</v>
@@ -4196,7 +4196,7 @@
     </row>
     <row r="302" ht="14.25">
       <c r="A302" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C302" s="5">
         <v>111112</v>
@@ -4207,7 +4207,7 @@
     </row>
     <row r="303" ht="14.25">
       <c r="A303" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C303" s="5">
         <v>111113</v>
@@ -4218,7 +4218,7 @@
     </row>
     <row r="304" ht="14.25">
       <c r="A304" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C304" s="5">
         <v>111114</v>
@@ -4229,7 +4229,7 @@
     </row>
     <row r="305" ht="14.25">
       <c r="A305" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C305" s="5">
         <v>111115</v>
@@ -4240,7 +4240,7 @@
     </row>
     <row r="306" ht="14.25">
       <c r="A306" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C306" s="5">
         <v>111116</v>
@@ -4251,7 +4251,7 @@
     </row>
     <row r="307" ht="14.25">
       <c r="A307" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C307" s="5">
         <v>111117</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="308" ht="14.25">
       <c r="A308" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C308" s="5">
         <v>111118</v>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="309" ht="14.25">
       <c r="A309" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C309" s="5">
         <v>111119</v>
@@ -4284,7 +4284,7 @@
     </row>
     <row r="310" ht="14.25">
       <c r="A310" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C310" s="5">
         <v>111120</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="311" ht="14.25">
       <c r="A311" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C311" s="5">
         <v>111121</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="316" ht="14.25">
       <c r="A316" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C316" s="5">
         <v>111126</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="317" ht="14.25">
       <c r="A317" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C317" s="5">
         <v>111127</v>
@@ -4405,7 +4405,7 @@
     </row>
     <row r="321" ht="14.25">
       <c r="A321" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C321" s="5">
         <v>111131</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="329" ht="14.25">
       <c r="A329" s="5" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C329" s="5">
         <v>111139</v>
@@ -4504,7 +4504,7 @@
     </row>
     <row r="330" ht="14.25">
       <c r="A330" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C330" s="5">
         <v>111140</v>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="331" ht="14.25">
       <c r="A331" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C331" s="5">
         <v>111141</v>
@@ -4526,7 +4526,7 @@
     </row>
     <row r="332" ht="14.25">
       <c r="A332" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C332" s="5">
         <v>111142</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="333" ht="14.25">
       <c r="A333" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C333" s="5">
         <v>111143</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="334" ht="14.25">
       <c r="A334" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C334" s="5">
         <v>111144</v>
@@ -4559,7 +4559,7 @@
     </row>
     <row r="335" ht="14.25">
       <c r="A335" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C335" s="5">
         <v>111145</v>
@@ -4570,7 +4570,7 @@
     </row>
     <row r="336" ht="14.25">
       <c r="A336" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C336" s="5">
         <v>111146</v>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="337" ht="14.25">
       <c r="A337" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C337" s="5">
         <v>111147</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="338" ht="14.25">
       <c r="A338" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C338" s="5">
         <v>111148</v>
@@ -4603,7 +4603,7 @@
     </row>
     <row r="339" ht="14.25">
       <c r="A339" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C339" s="5">
         <v>111149</v>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="340" ht="14.25">
       <c r="A340" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C340" s="5">
         <v>111150</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="341" ht="14.25">
       <c r="A341" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C341" s="5">
         <v>111151</v>
@@ -4636,7 +4636,7 @@
     </row>
     <row r="342" ht="14.25">
       <c r="A342" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C342" s="5">
         <v>111111</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="343" ht="14.25">
       <c r="A343" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C343" s="5">
         <v>111112</v>
@@ -4658,7 +4658,7 @@
     </row>
     <row r="344" ht="14.25">
       <c r="A344" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C344" s="5">
         <v>111113</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="345" ht="14.25">
       <c r="A345" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C345" s="5">
         <v>111114</v>
@@ -4680,7 +4680,7 @@
     </row>
     <row r="346" ht="14.25">
       <c r="A346" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C346" s="5">
         <v>111115</v>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="347" ht="14.25">
       <c r="A347" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C347" s="5">
         <v>111116</v>
@@ -4702,7 +4702,7 @@
     </row>
     <row r="348" ht="14.25">
       <c r="A348" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C348" s="5">
         <v>111117</v>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="349" ht="14.25">
       <c r="A349" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C349" s="5">
         <v>111118</v>
@@ -4724,7 +4724,7 @@
     </row>
     <row r="350" ht="14.25">
       <c r="A350" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C350" s="5">
         <v>111119</v>
@@ -4735,7 +4735,7 @@
     </row>
     <row r="351" ht="14.25">
       <c r="A351" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C351" s="5">
         <v>111120</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="352" ht="14.25">
       <c r="A352" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C352" s="5">
         <v>111121</v>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="353" ht="14.25">
       <c r="A353" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C353" s="5">
         <v>111122</v>
@@ -4768,7 +4768,7 @@
     </row>
     <row r="354" ht="14.25">
       <c r="A354" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C354" s="5">
         <v>111123</v>
@@ -4779,7 +4779,7 @@
     </row>
     <row r="355" ht="14.25">
       <c r="A355" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C355" s="5">
         <v>111124</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="356" ht="14.25">
       <c r="A356" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C356" s="5">
         <v>111125</v>
@@ -4801,7 +4801,7 @@
     </row>
     <row r="357" ht="14.25">
       <c r="A357" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C357" s="5">
         <v>111126</v>
@@ -4812,7 +4812,7 @@
     </row>
     <row r="358" ht="14.25">
       <c r="A358" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C358" s="5">
         <v>111127</v>
@@ -4823,7 +4823,7 @@
     </row>
     <row r="359" ht="14.25">
       <c r="A359" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C359" s="5">
         <v>111128</v>
@@ -4834,7 +4834,7 @@
     </row>
     <row r="360" ht="14.25">
       <c r="A360" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C360" s="5">
         <v>111129</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="361" ht="14.25">
       <c r="A361" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C361" s="5">
         <v>111130</v>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="362" ht="14.25">
       <c r="A362" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C362" s="5">
         <v>111131</v>
@@ -4867,7 +4867,7 @@
     </row>
     <row r="363" ht="14.25">
       <c r="A363" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C363" s="5">
         <v>111132</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="364" ht="14.25">
       <c r="A364" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C364" s="5">
         <v>111133</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="365" ht="14.25">
       <c r="A365" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C365" s="5">
         <v>111134</v>
@@ -4900,7 +4900,7 @@
     </row>
     <row r="366" ht="14.25">
       <c r="A366" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C366" s="5">
         <v>111135</v>
@@ -4911,7 +4911,7 @@
     </row>
     <row r="367" ht="14.25">
       <c r="A367" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C367" s="5">
         <v>111136</v>
@@ -4922,7 +4922,7 @@
     </row>
     <row r="368" ht="14.25">
       <c r="A368" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C368" s="5">
         <v>111137</v>
@@ -4933,7 +4933,7 @@
     </row>
     <row r="369" ht="14.25">
       <c r="A369" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C369" s="5">
         <v>111138</v>
@@ -4943,7 +4943,7 @@
       </c>
     </row>
     <row r="370" ht="14.25">
-      <c r="A370" s="4" t="s">
+      <c r="A370" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C370" s="5">
@@ -4955,7 +4955,7 @@
     </row>
     <row r="371" ht="14.25">
       <c r="A371" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C371" s="5">
         <v>111140</v>
@@ -4966,7 +4966,7 @@
     </row>
     <row r="372" ht="14.25">
       <c r="A372" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C372" s="5">
         <v>111141</v>
@@ -4977,7 +4977,7 @@
     </row>
     <row r="373" ht="14.25">
       <c r="A373" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C373" s="5">
         <v>111142</v>
@@ -4987,7 +4987,7 @@
       </c>
     </row>
     <row r="374" ht="14.25">
-      <c r="A374" s="6" t="s">
+      <c r="A374" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C374" s="5">
@@ -5032,7 +5032,7 @@
     </row>
     <row r="378" ht="14.25">
       <c r="A378" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C378" s="5">
         <v>111147</v>
@@ -5043,7 +5043,7 @@
     </row>
     <row r="379" ht="14.25">
       <c r="A379" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C379" s="5">
         <v>111148</v>
@@ -5087,7 +5087,7 @@
     </row>
     <row r="383" ht="14.25">
       <c r="A383" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C383">
         <v>123837</v>
@@ -5130,7 +5130,7 @@
       </c>
     </row>
     <row r="387" ht="14.25">
-      <c r="A387" s="4" t="s">
+      <c r="A387" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C387">
@@ -5141,7 +5141,7 @@
       </c>
     </row>
     <row r="388" ht="14.25">
-      <c r="A388" s="4" t="s">
+      <c r="A388" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C388">
@@ -5175,7 +5175,7 @@
     </row>
     <row r="391" ht="14.25">
       <c r="A391" s="5" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C391">
         <v>123845</v>
@@ -5186,7 +5186,7 @@
     </row>
     <row r="392" ht="14.25">
       <c r="A392" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C392">
         <v>123846</v>
@@ -5197,7 +5197,7 @@
     </row>
     <row r="393" ht="14.25">
       <c r="A393" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C393">
         <v>123847</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="394" ht="14.25">
       <c r="A394" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C394">
         <v>123848</v>
@@ -5219,7 +5219,7 @@
     </row>
     <row r="395" ht="14.25">
       <c r="A395" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C395">
         <v>123849</v>
@@ -5230,7 +5230,7 @@
     </row>
     <row r="396" ht="14.25">
       <c r="A396" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C396">
         <v>123850</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="397" ht="14.25">
       <c r="A397" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C397">
         <v>123851</v>
@@ -5252,7 +5252,7 @@
     </row>
     <row r="398" ht="14.25">
       <c r="A398" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C398">
         <v>123852</v>
@@ -5263,7 +5263,7 @@
     </row>
     <row r="399" ht="14.25">
       <c r="A399" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C399">
         <v>123853</v>
@@ -5274,7 +5274,7 @@
     </row>
     <row r="400" ht="14.25">
       <c r="A400" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C400">
         <v>123854</v>
@@ -5285,7 +5285,7 @@
     </row>
     <row r="401" ht="14.25">
       <c r="A401" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C401">
         <v>123855</v>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="402" ht="14.25">
       <c r="A402" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C402">
         <v>123856</v>
@@ -5307,7 +5307,7 @@
     </row>
     <row r="403" ht="14.25">
       <c r="A403" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C403">
         <v>123857</v>
@@ -5318,7 +5318,7 @@
     </row>
     <row r="404" ht="14.25">
       <c r="A404" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C404">
         <v>123858</v>
@@ -5329,7 +5329,7 @@
     </row>
     <row r="405" ht="14.25">
       <c r="A405" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C405">
         <v>123859</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="406" ht="14.25">
       <c r="A406" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C406">
         <v>123860</v>
@@ -5351,7 +5351,7 @@
     </row>
     <row r="407" ht="14.25">
       <c r="A407" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C407">
         <v>123861</v>
@@ -5362,7 +5362,7 @@
     </row>
     <row r="408" ht="14.25">
       <c r="A408" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C408">
         <v>123862</v>
@@ -5373,7 +5373,7 @@
     </row>
     <row r="409" ht="14.25">
       <c r="A409" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C409">
         <v>123863</v>
@@ -5384,7 +5384,7 @@
     </row>
     <row r="410" ht="14.25">
       <c r="A410" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C410">
         <v>123864</v>
@@ -5395,7 +5395,7 @@
     </row>
     <row r="411" ht="14.25">
       <c r="A411" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C411">
         <v>123865</v>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="412" ht="14.25">
       <c r="A412" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C412">
         <v>123866</v>
@@ -5417,7 +5417,7 @@
     </row>
     <row r="413" ht="14.25">
       <c r="A413" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C413">
         <v>123867</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="414" ht="14.25">
       <c r="A414" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C414">
         <v>123868</v>
@@ -5439,7 +5439,7 @@
     </row>
     <row r="415" ht="14.25">
       <c r="A415" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C415">
         <v>123869</v>
@@ -5450,7 +5450,7 @@
     </row>
     <row r="416" ht="14.25">
       <c r="A416" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C416">
         <v>123870</v>
@@ -5461,7 +5461,7 @@
     </row>
     <row r="417" ht="14.25">
       <c r="A417" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C417">
         <v>123871</v>
@@ -5472,7 +5472,7 @@
     </row>
     <row r="418" ht="14.25">
       <c r="A418" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C418">
         <v>123872</v>
@@ -5483,7 +5483,7 @@
     </row>
     <row r="419" ht="14.25">
       <c r="A419" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C419">
         <v>123873</v>
@@ -5494,7 +5494,7 @@
     </row>
     <row r="420" ht="14.25">
       <c r="A420" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C420">
         <v>123874</v>
@@ -5505,7 +5505,7 @@
     </row>
     <row r="421" ht="14.25">
       <c r="A421" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C421">
         <v>123875</v>
@@ -5516,7 +5516,7 @@
     </row>
     <row r="422" ht="14.25">
       <c r="A422" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C422">
         <v>123876</v>
@@ -5527,7 +5527,7 @@
     </row>
     <row r="423" ht="14.25">
       <c r="A423" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C423">
         <v>123877</v>
@@ -5538,7 +5538,7 @@
     </row>
     <row r="424" ht="14.25">
       <c r="A424" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C424">
         <v>123878</v>
@@ -5549,7 +5549,7 @@
     </row>
     <row r="425" ht="14.25">
       <c r="A425" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C425">
         <v>123879</v>
@@ -5560,7 +5560,7 @@
     </row>
     <row r="426" ht="14.25">
       <c r="A426" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C426">
         <v>123880</v>
@@ -5571,7 +5571,7 @@
     </row>
     <row r="427" ht="14.25">
       <c r="A427" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C427">
         <v>123881</v>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="428" ht="14.25">
       <c r="A428" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C428">
         <v>123882</v>
@@ -5593,7 +5593,7 @@
     </row>
     <row r="429" ht="14.25">
       <c r="A429" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C429">
         <v>123883</v>
@@ -5604,7 +5604,7 @@
     </row>
     <row r="430" ht="14.25">
       <c r="A430" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C430">
         <v>123884</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="431" ht="14.25">
       <c r="A431" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C431">
         <v>123885</v>
@@ -5626,7 +5626,7 @@
     </row>
     <row r="432" ht="14.25">
       <c r="A432" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C432">
         <v>123886</v>
@@ -5637,7 +5637,7 @@
     </row>
     <row r="433" ht="14.25">
       <c r="A433" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C433">
         <v>123887</v>
@@ -5648,7 +5648,7 @@
     </row>
     <row r="434" ht="14.25">
       <c r="A434" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C434">
         <v>123888</v>
@@ -5659,7 +5659,7 @@
     </row>
     <row r="435" ht="14.25">
       <c r="A435" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C435">
         <v>123889</v>

</xml_diff>